<commit_message>
got specific particle sizes in calibration experiments
</commit_message>
<xml_diff>
--- a/Hydrophones/Calibration/ManualRockMovements-1/mov1_calibration_curve_V1.xlsx
+++ b/Hydrophones/Calibration/ManualRockMovements-1/mov1_calibration_curve_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Hydrophones\Calibration\ManualRockMovements-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Calibration\ManualRockMovements-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5402F2A4-60C3-4456-B270-80B0258BA28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDBD82F-253B-40E3-BCE1-F7DECD73DDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Impact Pipe" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Particle #</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Raw Max A</t>
+  </si>
+  <si>
+    <t>B-axis (mm)</t>
+  </si>
+  <si>
+    <t>Sieve Size (mm)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1084,6 +1093,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1091,7 +1101,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1371,7 +1380,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Microphone!$F$2:$F$25</c:f>
+              <c:f>Microphone!$G$2:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1623,7 +1632,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Microphone!$E$2:$E$25</c:f>
+              <c:f>Microphone!$F$2:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2008,6 +2017,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2015,7 +2025,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3203,13 +3212,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>487680</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>480060</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>160974</xdr:rowOff>
@@ -4232,918 +4241,994 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160EE506-11C9-432A-9FE1-D04D59569C0D}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>167</v>
       </c>
       <c r="B2" s="2">
         <v>128</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
+        <v>220</v>
+      </c>
+      <c r="D2" s="1">
         <v>50</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>75</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>0.41399999999999998</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.42620000000000002</v>
       </c>
-      <c r="G2" s="1">
-        <f>D2-C2</f>
+      <c r="H2" s="1">
+        <f>E2-D2</f>
         <v>25</v>
       </c>
-      <c r="H2" s="1">
-        <f t="shared" ref="H2:H24" si="0">C3-D2</f>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I24" si="0">D3-E2</f>
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="K2">
-        <f>AVERAGE(H2:H24)</f>
+      <c r="L2">
+        <f>AVERAGE(I2:I24)</f>
         <v>26.913043478260871</v>
       </c>
-      <c r="P2">
-        <f>C2-'Impact Pipe'!C2</f>
+      <c r="Q2">
+        <f>D2-'Impact Pipe'!C2</f>
         <v>9</v>
       </c>
-      <c r="Q2">
-        <f>D2-'Impact Pipe'!D2</f>
+      <c r="R2">
+        <f>E2-'Impact Pipe'!D2</f>
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>128</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
         <v>90</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>110</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>0.49199999999999999</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.53100000000000003</v>
       </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:G25" si="1">D3-C3</f>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H25" si="1">E3-D3</f>
         <v>20</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P3">
-        <f>C3-'Impact Pipe'!C3</f>
+      <c r="Q3">
+        <f>D3-'Impact Pipe'!C3</f>
         <v>10</v>
       </c>
-      <c r="Q3">
-        <f>D3-'Impact Pipe'!D3</f>
+      <c r="R3">
+        <f>E3-'Impact Pipe'!D3</f>
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>128</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
+        <v>160</v>
+      </c>
+      <c r="D4" s="1">
         <v>130</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>140</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>0.63100000000000001</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>1.7165999999999999</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="P4">
-        <f>C4-'Impact Pipe'!C4</f>
+      <c r="Q4">
+        <f>D4-'Impact Pipe'!C4</f>
         <v>15</v>
       </c>
-      <c r="Q4">
-        <f>D4-'Impact Pipe'!D4</f>
+      <c r="R4">
+        <f>E4-'Impact Pipe'!D4</f>
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>168</v>
       </c>
       <c r="B5" s="2">
         <v>128</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
+        <v>196</v>
+      </c>
+      <c r="D5" s="1">
         <v>165</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>180</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>0.63100000000000001</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>2.181</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P5">
-        <f>C5-'Impact Pipe'!C5</f>
+      <c r="Q5">
+        <f>D5-'Impact Pipe'!C5</f>
         <v>15</v>
       </c>
-      <c r="Q5">
-        <f>D5-'Impact Pipe'!D5</f>
+      <c r="R5">
+        <f>E5-'Impact Pipe'!D5</f>
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>150</v>
       </c>
       <c r="B6" s="3">
         <v>90</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
+        <v>108.42</v>
+      </c>
+      <c r="D6" s="1">
         <v>200</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>215</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>0.19889999999999999</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>0.21290000000000001</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="P6">
-        <f>C6-'Impact Pipe'!C6</f>
+      <c r="Q6">
+        <f>D6-'Impact Pipe'!C6</f>
         <v>6</v>
       </c>
-      <c r="Q6">
-        <f>D6-'Impact Pipe'!D6</f>
+      <c r="R6">
+        <f>E6-'Impact Pipe'!D6</f>
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>90</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
+        <v>127.22</v>
+      </c>
+      <c r="D7" s="1">
         <v>240</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>250</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>0.43659999999999999</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>0.43819999999999998</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P7">
-        <f>C7-'Impact Pipe'!C7</f>
+      <c r="Q7">
+        <f>D7-'Impact Pipe'!C7</f>
         <v>14</v>
       </c>
-      <c r="Q7">
-        <f>D7-'Impact Pipe'!D7</f>
+      <c r="R7">
+        <f>E7-'Impact Pipe'!D7</f>
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>22</v>
       </c>
       <c r="B8" s="3">
         <v>90</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1">
         <v>280</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>286</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>0.45229999999999998</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>0.6008</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="P8">
-        <f>C8-'Impact Pipe'!C8</f>
+      <c r="Q8">
+        <f>D8-'Impact Pipe'!C8</f>
         <v>15</v>
       </c>
-      <c r="Q8">
-        <f>D8-'Impact Pipe'!D8</f>
+      <c r="R8">
+        <f>E8-'Impact Pipe'!D8</f>
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>152</v>
       </c>
       <c r="B9" s="3">
         <v>90</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
+        <v>91.54</v>
+      </c>
+      <c r="D9" s="1">
         <v>325</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>335</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>0.63100000000000001</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>1.6635</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P9">
-        <f>C9-'Impact Pipe'!C9</f>
+      <c r="Q9">
+        <f>D9-'Impact Pipe'!C9</f>
         <v>15</v>
       </c>
-      <c r="Q9">
-        <f>D9-'Impact Pipe'!D9</f>
+      <c r="R9">
+        <f>E9-'Impact Pipe'!D9</f>
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>12</v>
       </c>
       <c r="B10" s="4">
         <v>64</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
+        <v>84.2</v>
+      </c>
+      <c r="D10" s="1">
         <v>365</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>375</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>0.2351</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>0.25240000000000001</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="P10">
-        <f>C10-'Impact Pipe'!C10</f>
+      <c r="Q10">
+        <f>D10-'Impact Pipe'!C10</f>
         <v>8</v>
       </c>
-      <c r="Q10">
-        <f>D10-'Impact Pipe'!D10</f>
+      <c r="R10">
+        <f>E10-'Impact Pipe'!D10</f>
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>96</v>
       </c>
       <c r="B11" s="4">
         <v>64</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
+        <v>86.98</v>
+      </c>
+      <c r="D11" s="1">
         <v>400</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>415</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>0.39989999999999998</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>0.48759999999999998</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P11">
-        <f>C11-'Impact Pipe'!C11</f>
+      <c r="Q11">
+        <f>D11-'Impact Pipe'!C11</f>
         <v>8</v>
       </c>
-      <c r="Q11">
-        <f>D11-'Impact Pipe'!D11</f>
+      <c r="R11">
+        <f>E11-'Impact Pipe'!D11</f>
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>101</v>
       </c>
       <c r="B12" s="4">
         <v>64</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
+        <v>108.92</v>
+      </c>
+      <c r="D12" s="1">
         <v>445</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>450</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>0.1285</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>0.12859999999999999</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="P12">
-        <f>C12-'Impact Pipe'!C12</f>
+      <c r="Q12">
+        <f>D12-'Impact Pipe'!C12</f>
         <v>13</v>
       </c>
-      <c r="Q12">
-        <f>D12-'Impact Pipe'!D12</f>
+      <c r="R12">
+        <f>E12-'Impact Pipe'!D12</f>
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>24</v>
       </c>
       <c r="B13" s="4">
         <v>64</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
+        <v>87.98</v>
+      </c>
+      <c r="D13" s="1">
         <v>485</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>490</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>0.63100000000000001</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>1.5174000000000001</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P13">
-        <f>C13-'Impact Pipe'!C13</f>
+      <c r="Q13">
+        <f>D13-'Impact Pipe'!C13</f>
         <v>17</v>
       </c>
-      <c r="Q13">
-        <f>D13-'Impact Pipe'!D13</f>
+      <c r="R13">
+        <f>E13-'Impact Pipe'!D13</f>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>107</v>
       </c>
       <c r="B14" s="5">
         <v>45</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
+        <v>52.94</v>
+      </c>
+      <c r="D14" s="1">
         <v>520</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>540</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>0.16109999999999999</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>0.1636</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P14">
-        <f>C14-'Impact Pipe'!C14</f>
+      <c r="Q14">
+        <f>D14-'Impact Pipe'!C14</f>
         <v>5</v>
       </c>
-      <c r="Q14">
-        <f>D14-'Impact Pipe'!D14</f>
+      <c r="R14">
+        <f>E14-'Impact Pipe'!D14</f>
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>162</v>
       </c>
       <c r="B15" s="5">
         <v>45</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
+        <v>54.05</v>
+      </c>
+      <c r="D15" s="1">
         <v>570</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>575</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>0.29780000000000001</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>0.31130000000000002</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="P15">
-        <f>C15-'Impact Pipe'!C15</f>
+      <c r="Q15">
+        <f>D15-'Impact Pipe'!C15</f>
         <v>20</v>
       </c>
-      <c r="Q15">
-        <f>D15-'Impact Pipe'!D15</f>
+      <c r="R15">
+        <f>E15-'Impact Pipe'!D15</f>
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>159</v>
       </c>
       <c r="B16" s="5">
         <v>45</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="5">
+        <v>54.11</v>
+      </c>
+      <c r="D16" s="1">
         <v>610</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>625</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>7.6100000000000001E-2</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P16">
-        <f>C16-'Impact Pipe'!C16</f>
+      <c r="Q16">
+        <f>D16-'Impact Pipe'!C16</f>
         <v>15</v>
       </c>
-      <c r="Q16">
-        <f>D16-'Impact Pipe'!D16</f>
+      <c r="R16">
+        <f>E16-'Impact Pipe'!D16</f>
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>35</v>
       </c>
       <c r="B17" s="5">
         <v>45</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="5">
+        <v>64.849999999999994</v>
+      </c>
+      <c r="D17" s="1">
         <v>655</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>665</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>0.41970000000000002</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>0.42749999999999999</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P17">
-        <f>C17-'Impact Pipe'!C17</f>
+      <c r="Q17">
+        <f>D17-'Impact Pipe'!C17</f>
         <v>13</v>
       </c>
-      <c r="Q17">
-        <f>D17-'Impact Pipe'!D17</f>
+      <c r="R17">
+        <f>E17-'Impact Pipe'!D17</f>
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>69</v>
       </c>
       <c r="B18" s="6">
         <v>32</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1">
         <v>695</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>710</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>0.34360000000000002</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>0.34499999999999997</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P18">
-        <f>C18-'Impact Pipe'!C18</f>
+      <c r="Q18">
+        <f>D18-'Impact Pipe'!C18</f>
         <v>10</v>
       </c>
-      <c r="Q18">
-        <f>D18-'Impact Pipe'!D18</f>
+      <c r="R18">
+        <f>E18-'Impact Pipe'!D18</f>
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>85</v>
       </c>
       <c r="B19" s="6">
         <v>32</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="6">
+        <v>43.74</v>
+      </c>
+      <c r="D19" s="1">
         <v>740</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>760</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>5.1900000000000002E-2</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>6.4899999999999999E-2</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="P19">
-        <f>C19-'Impact Pipe'!C19</f>
+      <c r="Q19">
+        <f>D19-'Impact Pipe'!C19</f>
         <v>10</v>
       </c>
-      <c r="Q19">
-        <f>D19-'Impact Pipe'!D19</f>
+      <c r="R19">
+        <f>E19-'Impact Pipe'!D19</f>
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>61</v>
       </c>
       <c r="B20" s="6">
         <v>32</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1">
         <v>795</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>805</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.1132</v>
       </c>
       <c r="F20" s="1">
         <v>0.1132</v>
       </c>
       <c r="G20" s="1">
+        <v>0.1132</v>
+      </c>
+      <c r="H20" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="P20">
-        <f>C20-'Impact Pipe'!C20</f>
+      <c r="Q20">
+        <f>D20-'Impact Pipe'!C20</f>
         <v>13</v>
       </c>
-      <c r="Q20">
-        <f>D20-'Impact Pipe'!D20</f>
+      <c r="R20">
+        <f>E20-'Impact Pipe'!D20</f>
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>52</v>
       </c>
       <c r="B21" s="6">
         <v>32</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="6">
+        <v>45.6</v>
+      </c>
+      <c r="D21" s="1">
         <v>830</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>850</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>5.8500000000000003E-2</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>6.0400000000000002E-2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H21" s="1">
-        <f>C22-D21</f>
+      <c r="I21" s="1">
+        <f>D22-E21</f>
         <v>20</v>
       </c>
-      <c r="P21">
-        <f>C21-'Impact Pipe'!C21</f>
+      <c r="Q21">
+        <f>D21-'Impact Pipe'!C21</f>
         <v>10</v>
       </c>
-      <c r="Q21">
-        <f>D21-'Impact Pipe'!D21</f>
+      <c r="R21">
+        <f>E21-'Impact Pipe'!D21</f>
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>165</v>
       </c>
       <c r="B22" s="7">
         <v>16</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1">
         <v>870</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>900</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>7.4499999999999997E-2</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>8.1600000000000006E-2</v>
       </c>
-      <c r="G22" s="1">
-        <f>D22-C22</f>
+      <c r="H22" s="1">
+        <f>E22-D22</f>
         <v>30</v>
       </c>
-      <c r="H22" s="1">
-        <f>C23-D22</f>
+      <c r="I22" s="1">
+        <f>D23-E22</f>
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>166</v>
       </c>
       <c r="B23" s="7">
         <v>16</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1">
         <v>920</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>950</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>4.4299999999999999E-2</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>4.4699999999999997E-2</v>
       </c>
-      <c r="G23" s="1">
-        <f>D23-C23</f>
+      <c r="H23" s="1">
+        <f>E23-D23</f>
         <v>30</v>
       </c>
-      <c r="H23" s="1">
-        <f>C24-D23</f>
+      <c r="I23" s="1">
+        <f>D24-E23</f>
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>53</v>
       </c>
       <c r="B24" s="8">
         <v>22.6</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1">
         <v>970</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>1000</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>5.4300000000000001E-2</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P24">
-        <f>MIN(P2:P22)</f>
-        <v>5</v>
-      </c>
       <c r="Q24">
         <f>MIN(Q2:Q22)</f>
+        <v>5</v>
+      </c>
+      <c r="R24">
+        <f>MIN(R2:R22)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45</v>
       </c>
       <c r="B25" s="8">
         <v>22.6</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="8">
+        <v>29.55</v>
+      </c>
+      <c r="D25" s="1">
         <v>1020</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>1050</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>9.2200000000000004E-2</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>9.2799999999999994E-2</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="P25">
-        <f>AVERAGE(P2:P22)</f>
-        <v>12.05</v>
-      </c>
+      <c r="I25" s="1"/>
       <c r="Q25">
         <f>AVERAGE(Q2:Q22)</f>
+        <v>12.05</v>
+      </c>
+      <c r="R25">
+        <f>AVERAGE(R2:R22)</f>
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P26">
-        <f>MEDIAN(P2:P21)</f>
-        <v>13</v>
-      </c>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q26">
         <f>MEDIAN(Q2:Q21)</f>
+        <v>13</v>
+      </c>
+      <c r="R26">
+        <f>MEDIAN(R2:R21)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P27">
-        <f>MAX(P2:P21)</f>
-        <v>20</v>
-      </c>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q27">
         <f>MAX(Q2:Q21)</f>
+        <v>20</v>
+      </c>
+      <c r="R27">
+        <f>MAX(R2:R21)</f>
         <v>27</v>
       </c>
     </row>

</xml_diff>